<commit_message>
Début de la mise en place de la connection à la base de donnée
</commit_message>
<xml_diff>
--- a/InsertCard.xlsx
+++ b/InsertCard.xlsx
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E53" sqref="E2:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,8 +446,8 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <f>"sql = ""insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values ("&amp; ROW()-1 &amp;"," &amp; $A2 &amp; "," &amp; $B2 &amp; "," &amp; $C2 &amp; "," &amp;$D2&amp; ")"";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();"</f>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (1,As,CœurAs.png,Cœur,1)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <f>"sql = ""insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values ("&amp;ROW()-1&amp;","""&amp;$A2&amp;""","""&amp;$B2&amp;""","""&amp;$C2&amp;""","&amp;$D2&amp;")"";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();"</f>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (1,"As","CœurAs.png","Cœur",1)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -465,8 +465,8 @@
         <v>2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E53" si="1">"sql = ""insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values ("&amp; ROW()-1 &amp;"," &amp; $A3 &amp; "," &amp; $B3 &amp; "," &amp; $C3 &amp; "," &amp;$D3&amp; ")"";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();"</f>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (2,Deux,CœurDeux.png,Cœur,2)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <f t="shared" ref="E3:E53" si="1">"sql = ""insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values ("&amp;ROW()-1&amp;","""&amp;$A3&amp;""","""&amp;$B3&amp;""","""&amp;$C3&amp;""","&amp;$D3&amp;")"";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();"</f>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (2,"Deux","CœurDeux.png","Cœur",2)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -485,7 +485,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (3,Trois,CœurTrois.png,Cœur,3)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (3,"Trois","CœurTrois.png","Cœur",3)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (4,Quatre,CœurQuatre.png,Cœur,4)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (4,"Quatre","CœurQuatre.png","Cœur",4)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (5,Cinq,CœurCinq.png,Cœur,5)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (5,"Cinq","CœurCinq.png","Cœur",5)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (6,Six,CœurSix.png,Cœur,6)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (6,"Six","CœurSix.png","Cœur",6)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -561,7 +561,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (7,Sept,CœurSept.png,Cœur,7)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (7,"Sept","CœurSept.png","Cœur",7)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (8,Huit,CœurHuit.png,Cœur,8)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (8,"Huit","CœurHuit.png","Cœur",8)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,7 +599,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (9,Neuf,CœurNeuf.png,Cœur,9)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (9,"Neuf","CœurNeuf.png","Cœur",9)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -618,7 +618,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (10,Dix,CœurDix.png,Cœur,10)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (10,"Dix","CœurDix.png","Cœur",10)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (11,Valet,CœurValet.png,Cœur,11)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (11,"Valet","CœurValet.png","Cœur",11)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -656,7 +656,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (12,Dame,CœurDame.png,Cœur,12)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (12,"Dame","CœurDame.png","Cœur",12)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (13,Roi,CœurRoi.png,Cœur,13)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (13,"Roi","CœurRoi.png","Cœur",13)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (14,As,PiqueAs.png,Pique,1)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (14,"As","PiqueAs.png","Pique",1)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (15,Deux,PiqueDeux.png,Pique,2)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (15,"Deux","PiqueDeux.png","Pique",2)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (16,Trois,PiqueTrois.png,Pique,3)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (16,"Trois","PiqueTrois.png","Pique",3)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (17,Quatre,PiqueQuatre.png,Pique,4)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (17,"Quatre","PiqueQuatre.png","Pique",4)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -770,7 +770,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (18,Cinq,PiqueCinq.png,Pique,5)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (18,"Cinq","PiqueCinq.png","Pique",5)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (19,Six,PiqueSix.png,Pique,6)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (19,"Six","PiqueSix.png","Pique",6)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (20,Sept,PiqueSept.png,Pique,7)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (20,"Sept","PiqueSept.png","Pique",7)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (21,Huit,PiqueHuit.png,Pique,8)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (21,"Huit","PiqueHuit.png","Pique",8)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (22,Neuf,PiqueNeuf.png,Pique,9)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (22,"Neuf","PiqueNeuf.png","Pique",9)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -865,7 +865,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (23,Dix,PiqueDix.png,Pique,10)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (23,"Dix","PiqueDix.png","Pique",10)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -884,7 +884,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (24,Valet,PiqueValet.png,Pique,11)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (24,"Valet","PiqueValet.png","Pique",11)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (25,Dame,PiqueDame.png,Pique,12)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (25,"Dame","PiqueDame.png","Pique",12)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (26,Roi,PiqueRoi.png,Pique,13)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (26,"Roi","PiqueRoi.png","Pique",13)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -941,7 +941,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (27,As,CarreauAs.png,Carreau,1)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (27,"As","CarreauAs.png","Carreau",1)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (28,Deux,CarreauDeux.png,Carreau,2)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (28,"Deux","CarreauDeux.png","Carreau",2)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (29,Trois,CarreauTrois.png,Carreau,3)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (29,"Trois","CarreauTrois.png","Carreau",3)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (30,Quatre,CarreauQuatre.png,Carreau,4)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (30,"Quatre","CarreauQuatre.png","Carreau",4)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (31,Cinq,CarreauCinq.png,Carreau,5)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (31,"Cinq","CarreauCinq.png","Carreau",5)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (32,Six,CarreauSix.png,Carreau,6)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (32,"Six","CarreauSix.png","Carreau",6)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (33,Sept,CarreauSept.png,Carreau,7)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (33,"Sept","CarreauSept.png","Carreau",7)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (34,Huit,CarreauHuit.png,Carreau,8)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (34,"Huit","CarreauHuit.png","Carreau",8)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (35,Neuf,CarreauNeuf.png,Carreau,9)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (35,"Neuf","CarreauNeuf.png","Carreau",9)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (36,Dix,CarreauDix.png,Carreau,10)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (36,"Dix","CarreauDix.png","Carreau",10)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (37,Valet,CarreauValet.png,Carreau,11)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (37,"Valet","CarreauValet.png","Carreau",11)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (38,Dame,CarreauDame.png,Carreau,12)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (38,"Dame","CarreauDame.png","Carreau",12)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (39,Roi,CarreauRoi.png,Carreau,13)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (39,"Roi","CarreauRoi.png","Carreau",13)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (40,As,TrèfleAs.png,Trèfle,1)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (40,"As","TrèfleAs.png","Trèfle",1)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (41,Deux,TrèfleDeux.png,Trèfle,2)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (41,"Deux","TrèfleDeux.png","Trèfle",2)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (42,Trois,TrèfleTrois.png,Trèfle,3)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (42,"Trois","TrèfleTrois.png","Trèfle",3)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (43,Quatre,TrèfleQuatre.png,Trèfle,4)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (43,"Quatre","TrèfleQuatre.png","Trèfle",4)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (44,Cinq,TrèfleCinq.png,Trèfle,5)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (44,"Cinq","TrèfleCinq.png","Trèfle",5)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (45,Six,TrèfleSix.png,Trèfle,6)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (45,"Six","TrèfleSix.png","Trèfle",6)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1302,7 +1302,7 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (46,Sept,TrèfleSept.png,Trèfle,7)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (46,"Sept","TrèfleSept.png","Trèfle",7)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (47,Huit,TrèfleHuit.png,Trèfle,8)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (47,"Huit","TrèfleHuit.png","Trèfle",8)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (48,Neuf,TrèfleNeuf.png,Trèfle,9)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (48,"Neuf","TrèfleNeuf.png","Trèfle",9)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (49,Dix,TrèfleDix.png,Trèfle,10)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (49,"Dix","TrèfleDix.png","Trèfle",10)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,7 +1378,7 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (50,Valet,TrèfleValet.png,Trèfle,11)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (50,"Valet","TrèfleValet.png","Trèfle",11)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (51,Dame,TrèfleDame.png,Trèfle,12)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (51,"Dame","TrèfleDame.png","Trèfle",12)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="1"/>
-        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (52,Roi,TrèfleRoi.png,Trèfle,13)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
+        <v>sql = "insert into Card (IdCard, Name, LinkImage, Symbole, Valeur) values (52,"Roi","TrèfleRoi.png","Trèfle",13)";  command = new SQLiteCommand(sql, m_dbConnection); command.ExecuteNonQuery();</v>
       </c>
     </row>
   </sheetData>

</xml_diff>